<commit_message>
Added transactions to plot from desktop to github
</commit_message>
<xml_diff>
--- a/Stocks and Mutual Funds/Etrade Transactions.xlsx
+++ b/Stocks and Mutual Funds/Etrade Transactions.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RStudio\MyProjects\Stocks and Mutual Funds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5B4577A-2C49-45EF-BD71-773DC3C4AFCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF890449-FB81-403D-AD5F-DBF3F096F673}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4845" windowWidth="29040" windowHeight="15990" activeTab="2"/>
+    <workbookView xWindow="20370" yWindow="-4845" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
     <sheet name="DownloadTxnHistory (2)" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="196">
   <si>
     <t>TransactionDate</t>
   </si>
@@ -610,9 +618,6 @@
   </si>
   <si>
     <t>Sum of Amount</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Trans</t>
@@ -621,10 +626,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-409]d/mmm/yy;@"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1105,13 +1110,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1159,7 +1164,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-409]d/mmm/yy;@"/>
+      <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yy;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1175,12 +1180,12 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ken Harmon" refreshedDate="43969.910449305557" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="344">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ken Harmon" refreshedDate="43969.910449305557" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="344" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="11">
-    <cacheField name="TransactionDate" numFmtId="166">
+    <cacheField name="TransactionDate" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-11-01T00:00:00" maxDate="2020-05-14T00:00:00" count="51">
         <d v="2019-11-01T00:00:00"/>
         <d v="2019-11-04T00:00:00"/>
@@ -5112,10 +5117,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
-    <pivotField axis="axisRow" numFmtId="166" showAll="0">
+    <pivotField axis="axisRow" numFmtId="164" showAll="0">
       <items count="15">
         <item h="1" x="0"/>
         <item x="1"/>
@@ -5227,39 +5232,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I345" totalsRowShown="0">
-  <autoFilter ref="A1:I345"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I345" totalsRowShown="0">
+  <autoFilter ref="A1:I345" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I345">
     <sortCondition ref="B1:B345"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="TransactionDate" dataDxfId="0"/>
-    <tableColumn id="2" name="TransactionType"/>
-    <tableColumn id="3" name="SecurityType"/>
-    <tableColumn id="4" name="Symbol"/>
-    <tableColumn id="5" name="Quantity"/>
-    <tableColumn id="6" name="Amount"/>
-    <tableColumn id="7" name="Price"/>
-    <tableColumn id="8" name="Commission"/>
-    <tableColumn id="9" name="Description"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TransactionDate" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TransactionType"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SecurityType"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Symbol"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Quantity"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Amount"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Price"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Commission"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C308" totalsRowShown="0">
-  <autoFilter ref="A1:C308">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:C43" totalsRowShown="0">
+  <autoFilter ref="A1:C43" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C43">
+    <sortCondition ref="A1:A43"/>
+  </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Date"/>
-    <tableColumn id="2" name="Trans"/>
-    <tableColumn id="3" name="Amount"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Trans"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Amount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5561,7 +5563,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5668,7 +5670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M345"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5723,7 +5725,7 @@
         <v>185</v>
       </c>
       <c r="L1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -5857,15 +5859,15 @@
         <v>54</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K23" si="0">IF(A5=A6,"",A5)</f>
+        <f t="shared" ref="K5:K6" si="0">IF(A5=A6,"",A5)</f>
         <v/>
       </c>
       <c r="L5" t="str">
-        <f t="shared" ref="L5:L24" si="1">IF(A5=A6,"",B5)</f>
+        <f t="shared" ref="L5:L6" si="1">IF(A5=A6,"",B5)</f>
         <v/>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M35" si="2">IF(A5=A4,M4-F5,0-F5)</f>
+        <f t="shared" ref="M5:M6" si="2">IF(A5=A4,M4-F5,0-F5)</f>
         <v>500</v>
       </c>
     </row>
@@ -14887,15 +14889,15 @@
         <v>139</v>
       </c>
       <c r="K275">
-        <f t="shared" ref="K275:K277" si="11">IF(A275=A276,"",A275)</f>
+        <f t="shared" ref="K275" si="11">IF(A275=A276,"",A275)</f>
         <v>43895</v>
       </c>
       <c r="L275" t="str">
-        <f t="shared" ref="L275:L277" si="12">IF(A275=A276,"",B275)</f>
+        <f t="shared" ref="L275" si="12">IF(A275=A276,"",B275)</f>
         <v>Sold</v>
       </c>
       <c r="M275">
-        <f t="shared" ref="M275:M277" si="13">IF(A275=A274,M274+F275,0+F275)</f>
+        <f t="shared" ref="M275" si="13">IF(A275=A274,M274+F275,0+F275)</f>
         <v>200</v>
       </c>
     </row>
@@ -17335,11 +17337,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C308"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17353,2011 +17355,472 @@
         <v>185</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-    </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>43789</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>43802</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43789</v>
+        <v>43808</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>195</v>
+        <v>687.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>43809</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>500</v>
+        <v>99.99</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43802</v>
+        <v>43815</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>195</v>
+        <v>996.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>43816</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>118.35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>195</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>43817</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>231.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>195</v>
+        <v>485.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>43822</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C9">
-        <v>331.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>195</v>
+        <v>1766.37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>43822</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>431.75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>195</v>
+        <v>3299.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>43829</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>531.75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>195</v>
+        <v>600.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>43895</v>
       </c>
       <c r="B12" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C12">
-        <v>631.75</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>43808</v>
+        <v>43895</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C13">
-        <v>687.49</v>
+        <v>1976.28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>43809</v>
+        <v>43895</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14">
-        <v>99.99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>195</v>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>43896</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C15">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>195</v>
+        <v>575.11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>43896</v>
       </c>
       <c r="B16" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C16">
-        <v>800</v>
+        <v>5688.6299999999992</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>43815</v>
+        <v>43896</v>
       </c>
       <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>2567.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>43896</v>
+      </c>
+      <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C17">
-        <v>996.45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B18" t="s">
-        <v>195</v>
-      </c>
       <c r="C18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>195</v>
+        <v>4077.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>43899</v>
       </c>
       <c r="B19" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>200</v>
+        <v>7600</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>43816</v>
+        <v>43901</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>195</v>
+        <v>941.74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>43903</v>
       </c>
       <c r="B21" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C21">
-        <v>385.1</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>43817</v>
+        <v>43903</v>
       </c>
       <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>2548.94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>43903</v>
+      </c>
+      <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="C22">
-        <v>485.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>195</v>
-      </c>
-      <c r="B23" t="s">
-        <v>195</v>
-      </c>
       <c r="C23">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>195</v>
+        <v>1021.6700000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>43906</v>
       </c>
       <c r="B24" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C24">
-        <v>2499.9899999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>195</v>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>43906</v>
       </c>
       <c r="B25" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C25">
-        <v>3099.99</v>
+        <v>2046.95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>43822</v>
+        <v>43906</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C26">
-        <v>3299.99</v>
+        <v>3091.79</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>43829</v>
+        <v>43906</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27">
-        <v>600.02</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>195</v>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>43913</v>
       </c>
       <c r="B28" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>195</v>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>43916</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C29">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>195</v>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>43920</v>
       </c>
       <c r="B30" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C30">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>195</v>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>43921</v>
       </c>
       <c r="B31" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C31">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>195</v>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>43927</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C32">
-        <v>1100</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>43895</v>
+        <v>43929</v>
       </c>
       <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33">
+        <v>394.07</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>43929</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34">
+        <v>1000.34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>43929</v>
+      </c>
+      <c r="B35" t="s">
         <v>9</v>
       </c>
-      <c r="C33">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>195</v>
-      </c>
-      <c r="B34" t="s">
-        <v>195</v>
-      </c>
-      <c r="C34">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>195</v>
-      </c>
-      <c r="B35" t="s">
-        <v>195</v>
-      </c>
       <c r="C35">
-        <v>1677.79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>195</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>43934</v>
       </c>
       <c r="B36" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C36">
-        <v>2177.79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>195</v>
+        <v>260.78999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>43941</v>
       </c>
       <c r="B37" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C37">
-        <v>2677.79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>195</v>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>43948</v>
       </c>
       <c r="B38" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C38">
-        <v>2877.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>195</v>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>43951</v>
       </c>
       <c r="B39" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C39">
-        <v>3077.8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>195</v>
+        <v>110.21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>43959</v>
       </c>
       <c r="B40" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C40">
-        <v>3277.8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>195</v>
+        <v>1609.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>43963</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C41">
-        <v>3477.8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>195</v>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>43964</v>
       </c>
       <c r="B42" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="C42">
-        <v>3577.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>195</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>43964</v>
       </c>
       <c r="B43" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C43">
-        <v>3677.8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>195</v>
-      </c>
-      <c r="B44" t="s">
-        <v>195</v>
-      </c>
-      <c r="C44">
-        <v>3777.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>195</v>
-      </c>
-      <c r="B45" t="s">
-        <v>195</v>
-      </c>
-      <c r="C45">
-        <v>3877.8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>195</v>
-      </c>
-      <c r="B46" t="s">
-        <v>195</v>
-      </c>
-      <c r="C46">
-        <v>3977.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>43896</v>
-      </c>
-      <c r="B47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47">
-        <v>4077.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>195</v>
-      </c>
-      <c r="B48" t="s">
-        <v>195</v>
-      </c>
-      <c r="C48">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>195</v>
-      </c>
-      <c r="B49" t="s">
-        <v>195</v>
-      </c>
-      <c r="C49">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>195</v>
-      </c>
-      <c r="B50" t="s">
-        <v>195</v>
-      </c>
-      <c r="C50">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>195</v>
-      </c>
-      <c r="B51" t="s">
-        <v>195</v>
-      </c>
-      <c r="C51">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>195</v>
-      </c>
-      <c r="B52" t="s">
-        <v>195</v>
-      </c>
-      <c r="C52">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>195</v>
-      </c>
-      <c r="B53" t="s">
-        <v>195</v>
-      </c>
-      <c r="C53">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>195</v>
-      </c>
-      <c r="B54" t="s">
-        <v>195</v>
-      </c>
-      <c r="C54">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>195</v>
-      </c>
-      <c r="B55" t="s">
-        <v>195</v>
-      </c>
-      <c r="C55">
-        <v>7100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>195</v>
-      </c>
-      <c r="B56" t="s">
-        <v>195</v>
-      </c>
-      <c r="C56">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>195</v>
-      </c>
-      <c r="B57" t="s">
-        <v>195</v>
-      </c>
-      <c r="C57">
-        <v>7300</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>195</v>
-      </c>
-      <c r="B58" t="s">
-        <v>195</v>
-      </c>
-      <c r="C58">
-        <v>7400</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>195</v>
-      </c>
-      <c r="B59" t="s">
-        <v>195</v>
-      </c>
-      <c r="C59">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
-        <v>43899</v>
-      </c>
-      <c r="B60" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60">
-        <v>7600</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <v>43901</v>
-      </c>
-      <c r="B61" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61">
-        <v>941.74</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>195</v>
-      </c>
-      <c r="B62" t="s">
-        <v>195</v>
-      </c>
-      <c r="C62">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>195</v>
-      </c>
-      <c r="B63" t="s">
-        <v>195</v>
-      </c>
-      <c r="C63">
-        <v>821.67000000000007</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>195</v>
-      </c>
-      <c r="B64" t="s">
-        <v>195</v>
-      </c>
-      <c r="C64">
-        <v>921.67000000000007</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
-        <v>43903</v>
-      </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65">
-        <v>1021.6700000000001</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>195</v>
-      </c>
-      <c r="B66" t="s">
-        <v>195</v>
-      </c>
-      <c r="C66">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>195</v>
-      </c>
-      <c r="B67" t="s">
-        <v>195</v>
-      </c>
-      <c r="C67">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="5">
-        <v>43906</v>
-      </c>
-      <c r="B68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
-        <v>43913</v>
-      </c>
-      <c r="B69" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
-        <v>43916</v>
-      </c>
-      <c r="B70" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
-        <v>43920</v>
-      </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>195</v>
-      </c>
-      <c r="B72" t="s">
-        <v>195</v>
-      </c>
-      <c r="C72">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>195</v>
-      </c>
-      <c r="B73" t="s">
-        <v>195</v>
-      </c>
-      <c r="C73">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>195</v>
-      </c>
-      <c r="B74" t="s">
-        <v>195</v>
-      </c>
-      <c r="C74">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>195</v>
-      </c>
-      <c r="B75" t="s">
-        <v>195</v>
-      </c>
-      <c r="C75">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>195</v>
-      </c>
-      <c r="B76" t="s">
-        <v>195</v>
-      </c>
-      <c r="C76">
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
-        <v>43921</v>
-      </c>
-      <c r="B77" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
-        <v>43927</v>
-      </c>
-      <c r="B78" t="s">
-        <v>9</v>
-      </c>
-      <c r="C78">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>195</v>
-      </c>
-      <c r="B79" t="s">
-        <v>195</v>
-      </c>
-      <c r="C79">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="5">
-        <v>43929</v>
-      </c>
-      <c r="B80" t="s">
-        <v>9</v>
-      </c>
-      <c r="C80">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>195</v>
-      </c>
-      <c r="B81" t="s">
-        <v>195</v>
-      </c>
-      <c r="C81">
-        <v>160.79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
-        <v>43934</v>
-      </c>
-      <c r="B82" t="s">
-        <v>9</v>
-      </c>
-      <c r="C82">
-        <v>260.78999999999996</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="5">
-        <v>43941</v>
-      </c>
-      <c r="B83" t="s">
-        <v>9</v>
-      </c>
-      <c r="C83">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="5">
-        <v>43948</v>
-      </c>
-      <c r="B84" t="s">
-        <v>9</v>
-      </c>
-      <c r="C84">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
-        <v>43951</v>
-      </c>
-      <c r="B85" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85">
-        <v>110.21</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="5">
-        <v>43963</v>
-      </c>
-      <c r="B86" t="s">
-        <v>9</v>
-      </c>
-      <c r="C86">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>195</v>
-      </c>
-      <c r="B87" t="s">
-        <v>195</v>
-      </c>
-      <c r="C87">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>195</v>
-      </c>
-      <c r="B88" t="s">
-        <v>195</v>
-      </c>
-      <c r="C88">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>195</v>
-      </c>
-      <c r="B89" t="s">
-        <v>195</v>
-      </c>
-      <c r="C89">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>195</v>
-      </c>
-      <c r="B90" t="s">
-        <v>195</v>
-      </c>
-      <c r="C90">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>195</v>
-      </c>
-      <c r="B91" t="s">
-        <v>195</v>
-      </c>
-      <c r="C91">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>195</v>
-      </c>
-      <c r="B92" t="s">
-        <v>195</v>
-      </c>
-      <c r="C92">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>195</v>
-      </c>
-      <c r="B93" t="s">
-        <v>195</v>
-      </c>
-      <c r="C93">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>195</v>
-      </c>
-      <c r="B94" t="s">
-        <v>195</v>
-      </c>
-      <c r="C94">
-        <v>1850</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>195</v>
-      </c>
-      <c r="B95" t="s">
-        <v>195</v>
-      </c>
-      <c r="C95">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>195</v>
-      </c>
-      <c r="B96" t="s">
-        <v>195</v>
-      </c>
-      <c r="C96">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>195</v>
-      </c>
-      <c r="B97" t="s">
-        <v>195</v>
-      </c>
-      <c r="C97">
-        <v>2150</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>195</v>
-      </c>
-      <c r="B98" t="s">
-        <v>195</v>
-      </c>
-      <c r="C98">
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>195</v>
-      </c>
-      <c r="B99" t="s">
-        <v>195</v>
-      </c>
-      <c r="C99">
-        <v>2350</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>195</v>
-      </c>
-      <c r="B100" t="s">
-        <v>195</v>
-      </c>
-      <c r="C100">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>195</v>
-      </c>
-      <c r="B101" t="s">
-        <v>195</v>
-      </c>
-      <c r="C101">
-        <v>2550</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>195</v>
-      </c>
-      <c r="B102" t="s">
-        <v>195</v>
-      </c>
-      <c r="C102">
-        <v>2650</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="5">
-        <v>43964</v>
-      </c>
-      <c r="B103" t="s">
-        <v>9</v>
-      </c>
-      <c r="C103">
         <v>2750</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A104"/>
-    </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A105"/>
-    </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A106"/>
-    </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A107"/>
-    </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108"/>
-    </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A109"/>
-    </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A110"/>
-    </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111"/>
-    </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112"/>
-    </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113"/>
-    </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114"/>
-    </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115"/>
-    </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116"/>
-    </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117"/>
-    </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A118"/>
-    </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A119"/>
-    </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A120"/>
-    </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A121"/>
-    </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A122"/>
-    </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123"/>
-    </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A124"/>
-    </row>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125"/>
-    </row>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A126"/>
-    </row>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127"/>
-    </row>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A128"/>
-    </row>
-    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A129"/>
-    </row>
-    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A130"/>
-    </row>
-    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A131"/>
-    </row>
-    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A132"/>
-    </row>
-    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A133"/>
-    </row>
-    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A134"/>
-    </row>
-    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A135"/>
-    </row>
-    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136"/>
-    </row>
-    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A137"/>
-    </row>
-    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A138"/>
-    </row>
-    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A139"/>
-    </row>
-    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A140"/>
-    </row>
-    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A141"/>
-    </row>
-    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A142"/>
-    </row>
-    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A143"/>
-    </row>
-    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A144"/>
-    </row>
-    <row r="145" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A145"/>
-    </row>
-    <row r="146" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A146"/>
-    </row>
-    <row r="147" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A147"/>
-    </row>
-    <row r="148" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A148"/>
-    </row>
-    <row r="149" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A149"/>
-    </row>
-    <row r="150" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A150"/>
-    </row>
-    <row r="151" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A151"/>
-    </row>
-    <row r="152" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A152"/>
-    </row>
-    <row r="153" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A153"/>
-    </row>
-    <row r="154" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A154"/>
-    </row>
-    <row r="155" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A155"/>
-    </row>
-    <row r="156" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A156"/>
-    </row>
-    <row r="157" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A157"/>
-    </row>
-    <row r="158" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A158"/>
-    </row>
-    <row r="159" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A159"/>
-    </row>
-    <row r="160" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A160"/>
-    </row>
-    <row r="161" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A161"/>
-    </row>
-    <row r="162" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A162"/>
-    </row>
-    <row r="163" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A163"/>
-    </row>
-    <row r="164" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A164"/>
-    </row>
-    <row r="165" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A165"/>
-    </row>
-    <row r="166" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A166"/>
-    </row>
-    <row r="167" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A167"/>
-    </row>
-    <row r="168" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A168"/>
-    </row>
-    <row r="169" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A169"/>
-    </row>
-    <row r="170" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A170"/>
-    </row>
-    <row r="171" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A171"/>
-    </row>
-    <row r="172" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A172"/>
-    </row>
-    <row r="173" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A173"/>
-    </row>
-    <row r="174" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A174"/>
-    </row>
-    <row r="175" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A175"/>
-    </row>
-    <row r="176" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A176"/>
-    </row>
-    <row r="177" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A177"/>
-    </row>
-    <row r="178" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A178"/>
-    </row>
-    <row r="179" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A179"/>
-    </row>
-    <row r="180" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A180"/>
-    </row>
-    <row r="181" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A181"/>
-    </row>
-    <row r="182" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A182"/>
-    </row>
-    <row r="183" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A183"/>
-    </row>
-    <row r="184" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A184"/>
-    </row>
-    <row r="185" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A185"/>
-    </row>
-    <row r="186" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A186"/>
-    </row>
-    <row r="187" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A187"/>
-    </row>
-    <row r="188" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A188"/>
-    </row>
-    <row r="189" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A189"/>
-    </row>
-    <row r="190" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A190"/>
-    </row>
-    <row r="191" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A191"/>
-    </row>
-    <row r="192" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A192"/>
-    </row>
-    <row r="193" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A193"/>
-    </row>
-    <row r="194" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A194"/>
-    </row>
-    <row r="195" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A195"/>
-    </row>
-    <row r="196" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A196"/>
-    </row>
-    <row r="197" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A197"/>
-    </row>
-    <row r="198" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A198"/>
-    </row>
-    <row r="199" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A199"/>
-    </row>
-    <row r="200" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A200"/>
-    </row>
-    <row r="201" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A201"/>
-    </row>
-    <row r="202" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A202"/>
-    </row>
-    <row r="203" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A203"/>
-    </row>
-    <row r="204" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A204"/>
-    </row>
-    <row r="205" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A205"/>
-    </row>
-    <row r="206" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A206"/>
-    </row>
-    <row r="207" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A207"/>
-    </row>
-    <row r="208" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A208"/>
-    </row>
-    <row r="209" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A209"/>
-    </row>
-    <row r="210" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A210"/>
-    </row>
-    <row r="211" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A211"/>
-    </row>
-    <row r="212" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A212"/>
-    </row>
-    <row r="213" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A213"/>
-    </row>
-    <row r="214" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A214"/>
-    </row>
-    <row r="215" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A215"/>
-    </row>
-    <row r="216" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A216"/>
-    </row>
-    <row r="217" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A217"/>
-    </row>
-    <row r="218" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A218"/>
-    </row>
-    <row r="219" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A219"/>
-    </row>
-    <row r="220" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A220"/>
-    </row>
-    <row r="221" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A221"/>
-    </row>
-    <row r="222" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A222"/>
-    </row>
-    <row r="223" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A223"/>
-    </row>
-    <row r="224" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A224"/>
-    </row>
-    <row r="225" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A225"/>
-    </row>
-    <row r="226" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A226"/>
-    </row>
-    <row r="227" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A227"/>
-    </row>
-    <row r="228" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A228"/>
-    </row>
-    <row r="229" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A229"/>
-    </row>
-    <row r="230" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A230"/>
-    </row>
-    <row r="231" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A231"/>
-    </row>
-    <row r="232" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A232"/>
-    </row>
-    <row r="233" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A233"/>
-    </row>
-    <row r="234" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A234"/>
-    </row>
-    <row r="235" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A235"/>
-    </row>
-    <row r="236" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A236"/>
-    </row>
-    <row r="237" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A237"/>
-    </row>
-    <row r="238" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A238"/>
-    </row>
-    <row r="239" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A239"/>
-    </row>
-    <row r="240" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A240"/>
-    </row>
-    <row r="241" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A241"/>
-    </row>
-    <row r="242" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A242"/>
-    </row>
-    <row r="243" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A243"/>
-    </row>
-    <row r="244" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A244"/>
-    </row>
-    <row r="245" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A245"/>
-    </row>
-    <row r="246" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A246"/>
-    </row>
-    <row r="247" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A247"/>
-    </row>
-    <row r="248" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A248"/>
-    </row>
-    <row r="249" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A249"/>
-    </row>
-    <row r="250" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A250"/>
-    </row>
-    <row r="251" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A251"/>
-    </row>
-    <row r="252" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A252"/>
-    </row>
-    <row r="253" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A253"/>
-    </row>
-    <row r="254" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A254"/>
-    </row>
-    <row r="255" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A255"/>
-    </row>
-    <row r="256" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A256"/>
-    </row>
-    <row r="257" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A257"/>
-    </row>
-    <row r="258" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A258"/>
-    </row>
-    <row r="259" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A259"/>
-    </row>
-    <row r="260" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A260"/>
-    </row>
-    <row r="261" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A261"/>
-    </row>
-    <row r="262" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A262"/>
-    </row>
-    <row r="263" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A263"/>
-    </row>
-    <row r="264" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A264"/>
-    </row>
-    <row r="265" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A265"/>
-    </row>
-    <row r="266" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A266"/>
-    </row>
-    <row r="267" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A267"/>
-    </row>
-    <row r="268" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A268"/>
-    </row>
-    <row r="269" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A269"/>
-    </row>
-    <row r="270" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A270"/>
-    </row>
-    <row r="271" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A271"/>
-    </row>
-    <row r="272" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A272"/>
-    </row>
-    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A273"/>
-    </row>
-    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>195</v>
-      </c>
-      <c r="B274" t="s">
-        <v>195</v>
-      </c>
-      <c r="C274">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A275" s="5">
-        <v>43895</v>
-      </c>
-      <c r="B275" t="s">
-        <v>21</v>
-      </c>
-      <c r="C275">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
-        <v>195</v>
-      </c>
-      <c r="B276" t="s">
-        <v>195</v>
-      </c>
-      <c r="C276">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>195</v>
-      </c>
-      <c r="B277" t="s">
-        <v>195</v>
-      </c>
-      <c r="C277">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>195</v>
-      </c>
-      <c r="B278" t="s">
-        <v>195</v>
-      </c>
-      <c r="C278">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>195</v>
-      </c>
-      <c r="B279" t="s">
-        <v>195</v>
-      </c>
-      <c r="C279">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>195</v>
-      </c>
-      <c r="B280" t="s">
-        <v>195</v>
-      </c>
-      <c r="C280">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
-        <v>195</v>
-      </c>
-      <c r="B281" t="s">
-        <v>195</v>
-      </c>
-      <c r="C281">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>195</v>
-      </c>
-      <c r="B282" t="s">
-        <v>195</v>
-      </c>
-      <c r="C282">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>195</v>
-      </c>
-      <c r="B283" t="s">
-        <v>195</v>
-      </c>
-      <c r="C283">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
-        <v>195</v>
-      </c>
-      <c r="B284" t="s">
-        <v>195</v>
-      </c>
-      <c r="C284">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>195</v>
-      </c>
-      <c r="B285" t="s">
-        <v>195</v>
-      </c>
-      <c r="C285">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
-        <v>195</v>
-      </c>
-      <c r="B286" t="s">
-        <v>195</v>
-      </c>
-      <c r="C286">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
-        <v>195</v>
-      </c>
-      <c r="B287" t="s">
-        <v>195</v>
-      </c>
-      <c r="C287">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" s="5">
-        <v>43903</v>
-      </c>
-      <c r="B288" t="s">
-        <v>21</v>
-      </c>
-      <c r="C288">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>195</v>
-      </c>
-      <c r="B289" t="s">
-        <v>195</v>
-      </c>
-      <c r="C289">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>195</v>
-      </c>
-      <c r="B290" t="s">
-        <v>195</v>
-      </c>
-      <c r="C290">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>195</v>
-      </c>
-      <c r="B291" t="s">
-        <v>195</v>
-      </c>
-      <c r="C291">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A292" s="5">
-        <v>43906</v>
-      </c>
-      <c r="B292" t="s">
-        <v>21</v>
-      </c>
-      <c r="C292">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A293" s="5">
-        <v>43964</v>
-      </c>
-      <c r="B293" t="s">
-        <v>21</v>
-      </c>
-      <c r="C293">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A294" s="5">
-        <v>43929</v>
-      </c>
-      <c r="B294" t="s">
-        <v>21</v>
-      </c>
-      <c r="C294">
-        <v>394.07</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A295" s="5">
-        <v>43896</v>
-      </c>
-      <c r="B295" t="s">
-        <v>21</v>
-      </c>
-      <c r="C295">
-        <v>575.11</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>195</v>
-      </c>
-      <c r="B296" t="s">
-        <v>195</v>
-      </c>
-      <c r="C296">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A297" s="5">
-        <v>43959</v>
-      </c>
-      <c r="B297" t="s">
-        <v>21</v>
-      </c>
-      <c r="C297">
-        <v>1609.8</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A298" s="5">
-        <v>43929</v>
-      </c>
-      <c r="B298" t="s">
-        <v>21</v>
-      </c>
-      <c r="C298">
-        <v>1000.34</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>195</v>
-      </c>
-      <c r="B299" t="s">
-        <v>195</v>
-      </c>
-      <c r="C299">
-        <v>1133.07</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>195</v>
-      </c>
-      <c r="B300" t="s">
-        <v>195</v>
-      </c>
-      <c r="C300">
-        <v>2381.1899999999996</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
-        <v>195</v>
-      </c>
-      <c r="B301" t="s">
-        <v>195</v>
-      </c>
-      <c r="C301">
-        <v>3942.3599999999997</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A302" s="5">
-        <v>43896</v>
-      </c>
-      <c r="B302" t="s">
-        <v>21</v>
-      </c>
-      <c r="C302">
-        <v>5688.6299999999992</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A303" s="5">
-        <v>43822</v>
-      </c>
-      <c r="B303" t="s">
-        <v>21</v>
-      </c>
-      <c r="C303">
-        <v>1766.37</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A304" s="5">
-        <v>43895</v>
-      </c>
-      <c r="B304" t="s">
-        <v>21</v>
-      </c>
-      <c r="C304">
-        <v>1976.28</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A305" s="5">
-        <v>43906</v>
-      </c>
-      <c r="B305" t="s">
-        <v>21</v>
-      </c>
-      <c r="C305">
-        <v>2046.95</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A306" s="5">
-        <v>43903</v>
-      </c>
-      <c r="B306" t="s">
-        <v>21</v>
-      </c>
-      <c r="C306">
-        <v>2548.94</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A307" s="5">
-        <v>43896</v>
-      </c>
-      <c r="B307" t="s">
-        <v>21</v>
-      </c>
-      <c r="C307">
-        <v>2567.13</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A308" s="5">
-        <v>43906</v>
-      </c>
-      <c r="B308" t="s">
-        <v>21</v>
-      </c>
-      <c r="C308">
-        <v>3091.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>